<commit_message>
mise a jour des docs
</commit_message>
<xml_diff>
--- a/docs/mySoundsGantt.xlsx
+++ b/docs/mySoundsGantt.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RODRIGODCSTL\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\var\www\html\MySounds\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{649280EE-BFD1-4254-8A8E-6F4BE145409F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77BDB946-68F7-438C-B040-2A36F63B6E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{A29F5D2D-CC89-4920-B613-066EE70C1774}"/>
   </bookViews>
@@ -218,19 +218,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -258,6 +251,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -411,44 +410,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -461,9 +460,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="21" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="21" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="21" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -780,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8CA1C9-43DD-458B-B936-59F06ADC606F}">
   <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,10 +846,12 @@
         <v>2</v>
       </c>
       <c r="B2" s="27">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="C2" s="30">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D2" s="28"/>
       <c r="M2" s="17"/>
       <c r="P2" t="s">
         <v>53</v>
@@ -878,8 +883,15 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="E4" s="24"/>
+      <c r="B4" s="29">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E4" s="31">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F4" s="30">
+        <v>6.25E-2</v>
+      </c>
       <c r="M4" s="17"/>
     </row>
     <row r="5" spans="1:17" ht="21" x14ac:dyDescent="0.35">
@@ -903,23 +915,33 @@
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="E6" s="28"/>
+      <c r="B6" s="29">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E6" s="32">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="M6" s="17"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="E7" s="24"/>
+      <c r="B7" s="29">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E7" s="31">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="M7" s="17"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="12"/>
+      <c r="B8" s="29">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="M8" s="17"/>
     </row>
     <row r="9" spans="1:17" ht="21" x14ac:dyDescent="0.25">
@@ -943,63 +965,105 @@
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="29"/>
+      <c r="B10" s="29">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D10" s="31">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E10" s="33">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="M10" s="17"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
+      <c r="B11" s="29">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D11" s="33">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E11" s="33">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="M11" s="17"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
+      <c r="B12" s="29">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D12" s="33">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E12" s="33">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="M12" s="17"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
+      <c r="B13" s="29">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D13" s="31">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E13" s="31">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="M13" s="17"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="26"/>
+      <c r="B14" s="29">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D14" s="31">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E14" s="33">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="M14" s="17"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
+      <c r="B15" s="29">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D15" s="31">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E15" s="33">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="M15" s="17"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="26"/>
+      <c r="B16" s="29">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D16" s="31">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E16" s="33">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="M16" s="17"/>
     </row>
     <row r="17" spans="1:13" ht="21" x14ac:dyDescent="0.25">
@@ -1040,28 +1104,36 @@
       <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="12"/>
+      <c r="B19" s="29">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="M19" s="17"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="12"/>
+      <c r="B20" s="29">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="M20" s="17"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="12"/>
+      <c r="B21" s="29">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="M21" s="17"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="12"/>
+      <c r="B22" s="29">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="M22" s="17"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -1085,21 +1157,27 @@
       <c r="A24" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="12"/>
+      <c r="B24" s="29">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="M24" s="17"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="12"/>
+      <c r="B25" s="29">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="M25" s="17"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="12"/>
+      <c r="B26" s="29">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="M26" s="17"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -1334,10 +1412,21 @@
       <c r="A51" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="12"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="26"/>
+      <c r="B51" s="29">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C51" s="30">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D51" s="31">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="E51" s="30">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="F51" s="30">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="M51" s="17"/>
     </row>
     <row r="52" spans="1:13" ht="21" x14ac:dyDescent="0.25">
@@ -1375,7 +1464,7 @@
       <c r="M53" s="19"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>